<commit_message>
Reporting integrated with the code!
</commit_message>
<xml_diff>
--- a/framework-design/Resources/ModuleFiles/AmazonSmokeTest.xlsx
+++ b/framework-design/Resources/ModuleFiles/AmazonSmokeTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="47">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Value</t>
   </si>
   <si>
-    <t>Sample Script</t>
-  </si>
-  <si>
     <t>END</t>
   </si>
   <si>
@@ -66,12 +63,6 @@
     <t>i_URL</t>
   </si>
   <si>
-    <t>i_Action</t>
-  </si>
-  <si>
-    <t>Store</t>
-  </si>
-  <si>
     <t>Browser:i_BrowserName;@URL:i_URL</t>
   </si>
   <si>
@@ -97,6 +88,75 @@
   </si>
   <si>
     <t>CHROME</t>
+  </si>
+  <si>
+    <t>waitUntilObjectFound</t>
+  </si>
+  <si>
+    <t>Time:5</t>
+  </si>
+  <si>
+    <t>hoverOverObject</t>
+  </si>
+  <si>
+    <t>object_Click</t>
+  </si>
+  <si>
+    <t>setText</t>
+  </si>
+  <si>
+    <t>Text:i_UserName</t>
+  </si>
+  <si>
+    <t>Text:i_Password</t>
+  </si>
+  <si>
+    <t>hdr_Amazon</t>
+  </si>
+  <si>
+    <t>lnk_SignIn</t>
+  </si>
+  <si>
+    <t>btn_SignIn</t>
+  </si>
+  <si>
+    <t>lbl_Login</t>
+  </si>
+  <si>
+    <t>txt_UserName</t>
+  </si>
+  <si>
+    <t>txt_Password</t>
+  </si>
+  <si>
+    <t>btn_Login</t>
+  </si>
+  <si>
+    <t>i_UserName</t>
+  </si>
+  <si>
+    <t>i_Password</t>
+  </si>
+  <si>
+    <t>karthik.sharma041992@gmail.com</t>
+  </si>
+  <si>
+    <t>April@2018</t>
+  </si>
+  <si>
+    <t>Time:8</t>
+  </si>
+  <si>
+    <t>scriptPause</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Selects a product</t>
+  </si>
+  <si>
+    <t>Duration:4</t>
   </si>
 </sst>
 </file>
@@ -123,12 +183,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -144,7 +210,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -155,6 +221,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -474,21 +544,21 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -503,10 +573,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,7 +593,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>1</v>
@@ -532,25 +602,112 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
+        <v>20</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>4</v>
+      <c r="B3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -560,84 +717,100 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="36.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="I2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added a keyword for selecting dropdown values
</commit_message>
<xml_diff>
--- a/framework-design/Resources/ModuleFiles/AmazonSmokeTest.xlsx
+++ b/framework-design/Resources/ModuleFiles/AmazonSmokeTest.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="42">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>btn_Continue</t>
+  </si>
+  <si>
+    <t>karthik.sharma041992@gmail.com</t>
+  </si>
+  <si>
+    <t>April@2018</t>
   </si>
 </sst>
 </file>
@@ -651,7 +657,7 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:H3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -715,7 +721,12 @@
       <c r="F2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="5"/>
+      <c r="G2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="I2" s="5" t="s">
         <v>17</v>
       </c>
@@ -739,7 +750,12 @@
       <c r="F3" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="G3" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
@@ -748,8 +764,12 @@
   <hyperlinks>
     <hyperlink ref="I2" r:id="rId1"/>
     <hyperlink ref="I3" r:id="rId2"/>
+    <hyperlink ref="G2" r:id="rId3"/>
+    <hyperlink ref="G3" r:id="rId4"/>
+    <hyperlink ref="H2" r:id="rId5"/>
+    <hyperlink ref="H3" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId7"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made significant redesign to the function call structre. Introduced one function to initlize test step values and objects. Will soon implement error action functionality
</commit_message>
<xml_diff>
--- a/framework-design/Resources/ModuleFiles/AmazonSmokeTest.xlsx
+++ b/framework-design/Resources/ModuleFiles/AmazonSmokeTest.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="15120" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="15120" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ModuleConfig" sheetId="4" r:id="rId1"/>
@@ -63,9 +63,6 @@
     <t>i_Path</t>
   </si>
   <si>
-    <t>DocumentStamp</t>
-  </si>
-  <si>
     <t>Amazon Product Selection</t>
   </si>
   <si>
@@ -142,6 +139,9 @@
   </si>
   <si>
     <t>April@2018</t>
+  </si>
+  <si>
+    <t>ErrorAction</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,15 +578,15 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="1"/>
@@ -594,52 +594,52 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>35</v>
       </c>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -656,7 +656,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -681,7 +681,7 @@
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -693,10 +693,10 @@
         <v>13</v>
       </c>
       <c r="G1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" t="s">
         <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
       </c>
       <c r="I1" t="s">
         <v>14</v>
@@ -707,57 +707,57 @@
         <v>12</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H2" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="I2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
         <v>24</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>25</v>
       </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G3" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="H3" s="5" t="s">
-        <v>41</v>
-      </c>
       <c r="I3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>